<commit_message>
fixed integration mend concurrency
</commit_message>
<xml_diff>
--- a/LP GitHub Repos.xlsx
+++ b/LP GitHub Repos.xlsx
@@ -2029,11 +2029,7 @@
         </is>
       </c>
       <c r="H40" s="5" t="n"/>
-      <c r="I40" s="5" t="inlineStr">
-        <is>
-          <t>${{ github.workflow }}-${{ github.ref }}</t>
-        </is>
-      </c>
+      <c r="I40" s="5" t="n"/>
       <c r="J40" s="5" t="n"/>
     </row>
     <row r="41">
@@ -2753,11 +2749,7 @@
         </is>
       </c>
       <c r="H61" s="5" t="n"/>
-      <c r="I61" s="5" t="inlineStr">
-        <is>
-          <t>${{ github.workflow }}-${{ github.ref }}</t>
-        </is>
-      </c>
+      <c r="I61" s="5" t="n"/>
       <c r="J61" s="5" t="n"/>
     </row>
     <row r="62">
@@ -3125,11 +3117,7 @@
         </is>
       </c>
       <c r="H71" s="5" t="n"/>
-      <c r="I71" s="5" t="inlineStr">
-        <is>
-          <t>${{ github.workflow }}-${{ github.ref }}</t>
-        </is>
-      </c>
+      <c r="I71" s="5" t="n"/>
       <c r="J71" s="5" t="n"/>
     </row>
     <row r="72">

</xml_diff>

<commit_message>
fix syntax error from 'is' to '=='
</commit_message>
<xml_diff>
--- a/LP GitHub Repos.xlsx
+++ b/LP GitHub Repos.xlsx
@@ -776,11 +776,11 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="7" width="31.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="5.147857142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="28.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="18.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="6.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="20.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="32.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="20.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="7" width="8.43357142857143" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="7" width="25.719285714285714" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="7" width="27.433571428571426" customWidth="1" bestFit="1"/>

</xml_diff>